<commit_message>
some changes more to come
</commit_message>
<xml_diff>
--- a/Documents/Week 8/08_Team3WorkRequestRequirementsTraceabilityMatrixTemplate.xlsx
+++ b/Documents/Week 8/08_Team3WorkRequestRequirementsTraceabilityMatrixTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepo\UMGC_495_7381_Work_Request\Documents\Week 8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBCCB22-AEC4-4830-BF18-F37CFB62112C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3B5415-2E84-4342-A74F-5FB2B0F17BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,18 @@
     <definedName name="Text8" localSheetId="0">'Traceability Template'!#REF!</definedName>
     <definedName name="Text9" localSheetId="0">'Traceability Template'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -903,8 +914,8 @@
   </sheetPr>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>

</xml_diff>